<commit_message>
bug fixes, background image, sprite implementation
</commit_message>
<xml_diff>
--- a/Buerokratie/PM/timeLog.xlsx
+++ b/Buerokratie/PM/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktorija\Desktop\HTL\3. Klasse\SWP1\spielprojekt\Buerokratie\PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\Buerokratie\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FAD662-496D-475A-BA8B-5242E621D0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F41201E-FA8D-4BDA-A4C6-0E9E5133D6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>Begin</t>
   </si>
@@ -195,15 +195,19 @@
   </si>
   <si>
     <t>Bürokratie</t>
+  </si>
+  <si>
+    <t>player sprite implementation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;h&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -229,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -252,17 +256,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -275,14 +268,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -366,7 +359,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -392,6 +385,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -407,6 +405,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -422,6 +425,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -439,6 +447,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -464,13 +477,13 @@
             <c:numRef>
               <c:f>Tabelle1!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>#\ ##0.00\ "h"</c:formatCode>
+                <c:formatCode>#,##0.00\ "h"</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24.483333333333348</c:v>
+                  <c:v>27.65000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.950000000000045</c:v>
+                  <c:v>47.116666666666717</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.4166666666666607</c:v>
@@ -504,6 +517,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -519,6 +537,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -534,6 +557,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -551,6 +579,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-F689-4C9B-B8B2-116F3F9503F5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -579,16 +612,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.32471264367816094</c:v>
+                  <c:v>0.3382952691680261</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58289124668435033</c:v>
+                  <c:v>0.57646818923327914</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0%">
-                  <c:v>4.5313881520777963E-2</c:v>
+                  <c:v>4.1802610114192396E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0%">
-                  <c:v>4.7082228116710763E-2</c:v>
+                  <c:v>4.3433931484502336E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -645,7 +678,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -682,7 +715,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="LID4096"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1553,42 +1586,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA36"/>
+  <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="78" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="78" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="88.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="84.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.21875" customWidth="1"/>
-    <col min="18" max="18" width="11.77734375" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" customWidth="1"/>
-    <col min="21" max="21" width="23.33203125" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" customWidth="1"/>
-    <col min="23" max="23" width="13.21875" customWidth="1"/>
-    <col min="24" max="24" width="8.33203125" customWidth="1"/>
-    <col min="25" max="25" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.77734375" customWidth="1"/>
-    <col min="27" max="27" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="23.28515625" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" customWidth="1"/>
+    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" customWidth="1"/>
+    <col min="27" max="27" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="9"/>
       <c r="E1" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1635,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>31</v>
       </c>
@@ -1670,26 +1703,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4">
         <f>SUM(N3:N41)</f>
-        <v>24.483333333333348</v>
+        <v>27.65000000000002</v>
       </c>
       <c r="C3" s="5">
         <f>B3/B7</f>
-        <v>0.32471264367816094</v>
+        <v>0.3382952691680261</v>
       </c>
       <c r="E3" s="2">
         <v>45314</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="11">
         <f>8 + 45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="11">
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1703,11 +1736,11 @@
       <c r="K3" s="2">
         <v>45314</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="11">
         <f>8 + 45/60</f>
         <v>8.75</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="11">
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1721,15 +1754,15 @@
       <c r="Q3" s="2">
         <v>45344</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="11">
         <f>16+0/60</f>
         <v>16</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="11">
         <f>16+35/60</f>
         <v>16.583333333333332</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="8">
         <f t="shared" ref="T3:T8" si="2">S3-R3</f>
         <v>0.58333333333333215</v>
       </c>
@@ -1739,15 +1772,15 @@
       <c r="W3" s="2">
         <v>45344</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="11">
         <f>16+0/60</f>
         <v>16</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3" s="11">
         <f>16+35/60</f>
         <v>16.583333333333332</v>
       </c>
-      <c r="Z3" s="11">
+      <c r="Z3" s="8">
         <f t="shared" ref="Z3:Z8" si="3">Y3-X3</f>
         <v>0.58333333333333215</v>
       </c>
@@ -1755,26 +1788,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4">
         <f>SUM(H3:H64)</f>
-        <v>43.950000000000045</v>
+        <v>47.116666666666717</v>
       </c>
       <c r="C4" s="5">
         <f>B4/B7</f>
-        <v>0.58289124668435033</v>
+        <v>0.57646818923327914</v>
       </c>
       <c r="E4" s="2">
         <v>45314</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="11">
         <f>18+37/60</f>
         <v>18.616666666666667</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="11">
         <f>21 + 20/60</f>
         <v>21.333333333333332</v>
       </c>
@@ -1789,11 +1822,11 @@
       <c r="K4" s="2">
         <v>45315</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="11">
         <f t="shared" ref="M4:M11" si="4">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1807,15 +1840,15 @@
       <c r="Q4" s="2">
         <v>45351</v>
       </c>
-      <c r="R4" s="1">
-        <f t="shared" ref="R4:R8" si="5">16+0/60</f>
+      <c r="R4" s="11">
+        <f t="shared" ref="R4:R7" si="5">16+0/60</f>
         <v>16</v>
       </c>
-      <c r="S4" s="1">
-        <f t="shared" ref="S4:S8" si="6">16+35/60</f>
+      <c r="S4" s="11">
+        <f t="shared" ref="S4:S7" si="6">16+35/60</f>
         <v>16.583333333333332</v>
       </c>
-      <c r="T4" s="11">
+      <c r="T4" s="8">
         <f t="shared" si="2"/>
         <v>0.58333333333333215</v>
       </c>
@@ -1825,15 +1858,15 @@
       <c r="W4" s="2">
         <v>45351</v>
       </c>
-      <c r="X4" s="1">
-        <f t="shared" ref="X4:X8" si="7">16+0/60</f>
+      <c r="X4" s="11">
+        <f t="shared" ref="X4:X7" si="7">16+0/60</f>
         <v>16</v>
       </c>
-      <c r="Y4" s="1">
-        <f t="shared" ref="Y4:Y8" si="8">16+35/60</f>
+      <c r="Y4" s="11">
+        <f t="shared" ref="Y4:Y7" si="8">16+35/60</f>
         <v>16.583333333333332</v>
       </c>
-      <c r="Z4" s="11">
+      <c r="Z4" s="8">
         <f t="shared" si="3"/>
         <v>0.58333333333333215</v>
       </c>
@@ -1841,7 +1874,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1849,18 +1882,18 @@
         <f>SUM(T3:T77)</f>
         <v>3.4166666666666607</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <f>B5/B7</f>
-        <v>4.5313881520777963E-2</v>
+        <v>4.1802610114192396E-2</v>
       </c>
       <c r="E5" s="2">
         <v>45315</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="11">
         <f>11 + 10/60</f>
         <v>11.166666666666666</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="11">
         <f xml:space="preserve"> 13</f>
         <v>13</v>
       </c>
@@ -1874,11 +1907,11 @@
       <c r="K5" s="2">
         <v>45321</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="11">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="11">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -1892,15 +1925,15 @@
       <c r="Q5" s="2">
         <v>45358</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="11">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="11">
         <f t="shared" si="6"/>
         <v>16.583333333333332</v>
       </c>
-      <c r="T5" s="11">
+      <c r="T5" s="8">
         <f t="shared" si="2"/>
         <v>0.58333333333333215</v>
       </c>
@@ -1910,15 +1943,15 @@
       <c r="W5" s="2">
         <v>45358</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X5" s="11">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="Y5" s="11">
         <f t="shared" si="8"/>
         <v>16.583333333333332</v>
       </c>
-      <c r="Z5" s="11">
+      <c r="Z5" s="8">
         <f t="shared" si="3"/>
         <v>0.58333333333333215</v>
       </c>
@@ -1926,7 +1959,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1934,18 +1967,18 @@
         <f>SUM(Z3:Z95)</f>
         <v>3.5499999999999936</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <f>B6/B7</f>
-        <v>4.7082228116710763E-2</v>
+        <v>4.3433931484502336E-2</v>
       </c>
       <c r="E6" s="2">
         <v>45315</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="11">
         <f xml:space="preserve"> 17 + 30/60</f>
         <v>17.5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="11">
         <f>18 + 40/60</f>
         <v>18.666666666666668</v>
       </c>
@@ -1959,10 +1992,10 @@
       <c r="K6" s="2">
         <v>45322</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="11">
         <v>8</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="11">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -1976,15 +2009,15 @@
       <c r="Q6" s="2">
         <v>45358</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="11">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="11">
         <f t="shared" si="6"/>
         <v>16.583333333333332</v>
       </c>
-      <c r="T6" s="11">
+      <c r="T6" s="8">
         <f t="shared" si="2"/>
         <v>0.58333333333333215</v>
       </c>
@@ -1994,15 +2027,15 @@
       <c r="W6" s="2">
         <v>45358</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="11">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Y6" s="11">
         <f t="shared" si="8"/>
         <v>16.583333333333332</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6" s="8">
         <f t="shared" si="3"/>
         <v>0.58333333333333215</v>
       </c>
@@ -2010,26 +2043,26 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="4">
         <f>SUM(B3:B6)</f>
-        <v>75.400000000000048</v>
-      </c>
-      <c r="C7" s="8">
+        <v>81.733333333333391</v>
+      </c>
+      <c r="C7" s="6">
         <f>SUM(C3:C6)</f>
         <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>45316</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="11">
         <f>19+42/60</f>
         <v>19.7</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="11">
         <f xml:space="preserve"> 21 + 30/60</f>
         <v>21.5</v>
       </c>
@@ -2043,10 +2076,10 @@
       <c r="K7" s="2">
         <v>45335</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="11">
         <v>8</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="11">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2060,15 +2093,15 @@
       <c r="Q7" s="2">
         <v>45365</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="11">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="11">
         <f t="shared" si="6"/>
         <v>16.583333333333332</v>
       </c>
-      <c r="T7" s="11">
+      <c r="T7" s="8">
         <f t="shared" si="2"/>
         <v>0.58333333333333215</v>
       </c>
@@ -2078,15 +2111,15 @@
       <c r="W7" s="2">
         <v>45365</v>
       </c>
-      <c r="X7" s="1">
+      <c r="X7" s="11">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="Y7" s="11">
         <f t="shared" si="8"/>
         <v>16.583333333333332</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Z7" s="8">
         <f t="shared" si="3"/>
         <v>0.58333333333333215</v>
       </c>
@@ -2094,15 +2127,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E8" s="2">
         <v>45321</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="11">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2116,10 +2149,10 @@
       <c r="K8" s="2">
         <v>45336</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="11">
         <v>8</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="11">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2133,15 +2166,15 @@
       <c r="Q8" s="2">
         <v>45393</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="11">
         <f>18+45/60</f>
         <v>18.75</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="11">
         <f>19+15/60</f>
         <v>19.25</v>
       </c>
-      <c r="T8" s="11">
+      <c r="T8" s="8">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
@@ -2151,15 +2184,15 @@
       <c r="W8" s="2">
         <v>45393</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="11">
         <f>19+15/60</f>
         <v>19.25</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="Y8" s="11">
         <f>19+53/60</f>
         <v>19.883333333333333</v>
       </c>
-      <c r="Z8" s="11">
+      <c r="Z8" s="8">
         <f t="shared" si="3"/>
         <v>0.63333333333333286</v>
       </c>
@@ -2167,15 +2200,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E9" s="2">
         <v>45322</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="11">
         <f>14+45/60</f>
         <v>14.75</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="11">
         <f>16+40/60</f>
         <v>16.666666666666668</v>
       </c>
@@ -2189,11 +2222,11 @@
       <c r="K9" s="2">
         <v>45342</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="11">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2215,14 +2248,14 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E10" s="2">
         <v>45323</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="11">
         <v>8</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2236,11 +2269,11 @@
       <c r="K10" s="2">
         <v>45343</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="11">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2262,15 +2295,15 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E11" s="2">
         <v>45323</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="11">
         <f>17+35/60</f>
         <v>17.583333333333332</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="11">
         <f>19</f>
         <v>19</v>
       </c>
@@ -2284,11 +2317,11 @@
       <c r="K11" s="2">
         <v>45349</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="11">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2310,15 +2343,15 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E12" s="2">
         <v>45324</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="11">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2332,10 +2365,10 @@
       <c r="K12" s="2">
         <v>45356</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="11">
         <v>8</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="11">
         <f t="shared" ref="M12:M18" si="9">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2357,15 +2390,15 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E13" s="2">
         <v>45324</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="11">
         <f>13+53/60</f>
         <v>13.883333333333333</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="11">
         <f>14+36/60</f>
         <v>14.6</v>
       </c>
@@ -2379,11 +2412,11 @@
       <c r="K13" s="2">
         <v>45363</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="11">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2405,15 +2438,15 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E14" s="2">
         <v>45326</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="11">
         <f xml:space="preserve"> 18+30/60</f>
         <v>18.5</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="11">
         <f>19+42/60</f>
         <v>19.7</v>
       </c>
@@ -2427,11 +2460,11 @@
       <c r="K14" s="2">
         <v>45384</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="11">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2453,15 +2486,15 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E15" s="2">
         <v>45334</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="11">
         <f>12+53/60</f>
         <v>12.883333333333333</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="11">
         <f>13+7/60</f>
         <v>13.116666666666667</v>
       </c>
@@ -2475,11 +2508,11 @@
       <c r="K15" s="2">
         <v>45385</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="11">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2501,15 +2534,15 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E16" s="2">
         <v>45334</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="11">
         <f>10+21/60</f>
         <v>10.35</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="11">
         <f>10+42/60</f>
         <v>10.7</v>
       </c>
@@ -2523,11 +2556,11 @@
       <c r="K16" s="2">
         <v>45391</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="11">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2549,14 +2582,14 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E17" s="2">
         <v>45335</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="11">
         <v>8</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2570,11 +2603,11 @@
       <c r="K17" s="2">
         <v>45392</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="11">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2596,15 +2629,15 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E18" s="2">
         <v>45335</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="11">
         <f>14+32/60</f>
         <v>14.533333333333333</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="11">
         <f>15 + 10/60</f>
         <v>15.166666666666666</v>
       </c>
@@ -2618,11 +2651,11 @@
       <c r="K18" s="2">
         <v>45399</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="11">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2644,15 +2677,15 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E19" s="2">
         <v>45335</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="11">
         <f>17+35/60</f>
         <v>17.583333333333332</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="11">
         <f>17+47/60</f>
         <v>17.783333333333335</v>
       </c>
@@ -2666,11 +2699,11 @@
       <c r="K19" s="2">
         <v>45399</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L19" s="11">
         <f>20+33/60</f>
         <v>20.55</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="11">
         <f>21+12/60</f>
         <v>21.2</v>
       </c>
@@ -2692,14 +2725,14 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E20" s="2">
         <v>45336</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="11">
         <v>8</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2708,14 +2741,24 @@
         <v>1.5833333333333339</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="K20" s="2">
+        <v>45405</v>
+      </c>
+      <c r="L20" s="11">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M20" s="11">
+        <f t="shared" ref="M20:M21" si="13">9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="N20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="1"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -2727,15 +2770,15 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E21" s="2">
         <v>45342</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2746,14 +2789,24 @@
       <c r="I21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="K21" s="2">
+        <v>45406</v>
+      </c>
+      <c r="L21" s="11">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M21" s="11">
+        <f t="shared" si="13"/>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="N21" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="1"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -2765,15 +2818,15 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E22" s="2">
         <v>45343</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2803,15 +2856,15 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E23" s="2">
         <v>45349</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2839,15 +2892,15 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E24" s="2">
         <v>45350</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="11">
         <f>18+24/60</f>
         <v>18.399999999999999</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="11">
         <f>20+21/60</f>
         <v>20.350000000000001</v>
       </c>
@@ -2875,15 +2928,15 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E25" s="2">
         <v>45352</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="11">
         <f>14+54/60</f>
         <v>14.9</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="11">
         <f>16+22/60</f>
         <v>16.366666666666667</v>
       </c>
@@ -2894,17 +2947,21 @@
       <c r="I25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="6"/>
-    </row>
-    <row r="26" spans="5:27" x14ac:dyDescent="0.3">
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E26" s="2">
         <v>45356</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2915,208 +2972,310 @@
       <c r="I26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N26" s="6"/>
-    </row>
-    <row r="27" spans="5:27" x14ac:dyDescent="0.3">
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E27" s="2">
         <v>45357</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="11">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" ref="H27:H34" si="13">G27-F27</f>
+        <f t="shared" ref="H27:H34" si="14">G27-F27</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N27" s="6"/>
-    </row>
-    <row r="28" spans="5:27" x14ac:dyDescent="0.3">
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E28" s="2">
         <v>45357</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="11">
         <f>17+54/60</f>
         <v>17.899999999999999</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="11">
         <f>18+31/60</f>
         <v>18.516666666666666</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.61666666666666714</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="5:27" x14ac:dyDescent="0.3">
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E29" s="2">
         <v>45359</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="11">
         <f>15+53/60</f>
         <v>15.883333333333333</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="11">
         <f>16+29/60</f>
         <v>16.483333333333334</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E30" s="2">
         <v>45361</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="11">
         <f>16+42/60</f>
         <v>16.7</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="11">
         <f>17+10/60</f>
         <v>17.166666666666668</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.46666666666666856</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E31" s="2">
         <v>45363</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G31" s="1">
-        <f t="shared" ref="G31:G36" si="14">9+35/60</f>
+      <c r="G31" s="11">
+        <f t="shared" ref="G31:G38" si="15">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="5:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:27" x14ac:dyDescent="0.25">
       <c r="E32" s="2">
         <v>45384</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="11">
+        <f t="shared" si="15"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H32" s="3">
         <f t="shared" si="14"/>
-        <v>9.5833333333333339</v>
-      </c>
-      <c r="H32" s="3">
-        <f t="shared" si="13"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E33" s="6">
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="2">
         <v>45385</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="11">
+        <f t="shared" si="15"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H33" s="3">
         <f t="shared" si="14"/>
-        <v>9.5833333333333339</v>
-      </c>
-      <c r="H33" s="3">
-        <f t="shared" si="13"/>
         <v>1.5833333333333339</v>
       </c>
-      <c r="I33" s="7" t="s">
+      <c r="I33" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E34" s="6">
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" s="2">
         <v>45391</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="11">
+        <f t="shared" si="15"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H34" s="3">
         <f t="shared" si="14"/>
-        <v>9.5833333333333339</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="13"/>
         <v>1.5833333333333339</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="I34" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E35" s="6">
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="2">
         <v>45392</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G35" s="1">
-        <f t="shared" si="14"/>
+      <c r="G35" s="11">
+        <f t="shared" si="15"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" ref="H35" si="15">G35-F35</f>
+        <f t="shared" ref="H35" si="16">G35-F35</f>
         <v>1.5833333333333339</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E36" s="6">
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="2">
         <v>45399</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="11">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G36" s="1">
-        <f t="shared" si="14"/>
+      <c r="G36" s="11">
+        <f t="shared" si="15"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" ref="H36" si="16">G36-F36</f>
+        <f t="shared" ref="H36" si="17">G36-F36</f>
         <v>1.5833333333333339</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I36" s="1" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="2">
+        <v>45405</v>
+      </c>
+      <c r="F37" s="11">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G37" s="11">
+        <f t="shared" si="15"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H37" s="3">
+        <f t="shared" ref="H37:H38" si="18">G37-F37</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="2">
+        <v>45406</v>
+      </c>
+      <c r="F38" s="11">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G38" s="11">
+        <f t="shared" si="15"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H38" s="3">
+        <f t="shared" si="18"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:I25">

</xml_diff>

<commit_message>
tries counter and Restart (work in progress)
</commit_message>
<xml_diff>
--- a/Buerokratie/PM/timeLog.xlsx
+++ b/Buerokratie/PM/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\Buerokratie\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F41201E-FA8D-4BDA-A4C6-0E9E5133D6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C395D3-6FD5-4C72-B5A7-579C1EF9123A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>Begin</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>player sprite implementation</t>
+  </si>
+  <si>
+    <t>lil fixes</t>
+  </si>
+  <si>
+    <t>tries counter</t>
   </si>
 </sst>
 </file>
@@ -207,7 +213,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;h&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -261,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -271,11 +277,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -480,10 +485,10 @@
                 <c:formatCode>#,##0.00\ "h"</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>27.65000000000002</c:v>
+                  <c:v>30.816666666666691</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.116666666666717</c:v>
+                  <c:v>50.283333333333388</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.4166666666666607</c:v>
@@ -612,16 +617,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.3382952691680261</c:v>
+                  <c:v>0.34992429977289935</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57646818923327914</c:v>
+                  <c:v>0.57096896290688892</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0%">
-                  <c:v>4.1802610114192396E-2</c:v>
+                  <c:v>3.8796366389099071E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0%">
-                  <c:v>4.3433931484502336E-2</c:v>
+                  <c:v>4.0310370931112692E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="78" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,10 +1623,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="10"/>
       <c r="E1" t="s">
         <v>3</v>
       </c>
@@ -1709,20 +1714,20 @@
       </c>
       <c r="B3" s="4">
         <f>SUM(N3:N41)</f>
-        <v>27.65000000000002</v>
+        <v>30.816666666666691</v>
       </c>
       <c r="C3" s="5">
         <f>B3/B7</f>
-        <v>0.3382952691680261</v>
+        <v>0.34992429977289935</v>
       </c>
       <c r="E3" s="2">
         <v>45314</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <f>8 + 45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1736,11 +1741,11 @@
       <c r="K3" s="2">
         <v>45314</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="9">
         <f>8 + 45/60</f>
         <v>8.75</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="9">
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1754,11 +1759,11 @@
       <c r="Q3" s="2">
         <v>45344</v>
       </c>
-      <c r="R3" s="11">
+      <c r="R3" s="9">
         <f>16+0/60</f>
         <v>16</v>
       </c>
-      <c r="S3" s="11">
+      <c r="S3" s="9">
         <f>16+35/60</f>
         <v>16.583333333333332</v>
       </c>
@@ -1772,11 +1777,11 @@
       <c r="W3" s="2">
         <v>45344</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="9">
         <f>16+0/60</f>
         <v>16</v>
       </c>
-      <c r="Y3" s="11">
+      <c r="Y3" s="9">
         <f>16+35/60</f>
         <v>16.583333333333332</v>
       </c>
@@ -1794,20 +1799,20 @@
       </c>
       <c r="B4" s="4">
         <f>SUM(H3:H64)</f>
-        <v>47.116666666666717</v>
+        <v>50.283333333333388</v>
       </c>
       <c r="C4" s="5">
         <f>B4/B7</f>
-        <v>0.57646818923327914</v>
+        <v>0.57096896290688892</v>
       </c>
       <c r="E4" s="2">
         <v>45314</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <f>18+37/60</f>
         <v>18.616666666666667</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <f>21 + 20/60</f>
         <v>21.333333333333332</v>
       </c>
@@ -1822,11 +1827,11 @@
       <c r="K4" s="2">
         <v>45315</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="9">
         <f t="shared" ref="M4:M11" si="4">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1840,11 +1845,11 @@
       <c r="Q4" s="2">
         <v>45351</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="9">
         <f t="shared" ref="R4:R7" si="5">16+0/60</f>
         <v>16</v>
       </c>
-      <c r="S4" s="11">
+      <c r="S4" s="9">
         <f t="shared" ref="S4:S7" si="6">16+35/60</f>
         <v>16.583333333333332</v>
       </c>
@@ -1858,11 +1863,11 @@
       <c r="W4" s="2">
         <v>45351</v>
       </c>
-      <c r="X4" s="11">
+      <c r="X4" s="9">
         <f t="shared" ref="X4:X7" si="7">16+0/60</f>
         <v>16</v>
       </c>
-      <c r="Y4" s="11">
+      <c r="Y4" s="9">
         <f t="shared" ref="Y4:Y7" si="8">16+35/60</f>
         <v>16.583333333333332</v>
       </c>
@@ -1884,16 +1889,16 @@
       </c>
       <c r="C5" s="7">
         <f>B5/B7</f>
-        <v>4.1802610114192396E-2</v>
+        <v>3.8796366389099071E-2</v>
       </c>
       <c r="E5" s="2">
         <v>45315</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <f>11 + 10/60</f>
         <v>11.166666666666666</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <f xml:space="preserve"> 13</f>
         <v>13</v>
       </c>
@@ -1907,11 +1912,11 @@
       <c r="K5" s="2">
         <v>45321</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="9">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="9">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -1925,11 +1930,11 @@
       <c r="Q5" s="2">
         <v>45358</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="9">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="S5" s="11">
+      <c r="S5" s="9">
         <f t="shared" si="6"/>
         <v>16.583333333333332</v>
       </c>
@@ -1943,11 +1948,11 @@
       <c r="W5" s="2">
         <v>45358</v>
       </c>
-      <c r="X5" s="11">
+      <c r="X5" s="9">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="Y5" s="11">
+      <c r="Y5" s="9">
         <f t="shared" si="8"/>
         <v>16.583333333333332</v>
       </c>
@@ -1969,16 +1974,16 @@
       </c>
       <c r="C6" s="7">
         <f>B6/B7</f>
-        <v>4.3433931484502336E-2</v>
+        <v>4.0310370931112692E-2</v>
       </c>
       <c r="E6" s="2">
         <v>45315</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <f xml:space="preserve"> 17 + 30/60</f>
         <v>17.5</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <f>18 + 40/60</f>
         <v>18.666666666666668</v>
       </c>
@@ -1992,10 +1997,10 @@
       <c r="K6" s="2">
         <v>45322</v>
       </c>
-      <c r="L6" s="11">
-        <v>8</v>
-      </c>
-      <c r="M6" s="11">
+      <c r="L6" s="9">
+        <v>8</v>
+      </c>
+      <c r="M6" s="9">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2009,11 +2014,11 @@
       <c r="Q6" s="2">
         <v>45358</v>
       </c>
-      <c r="R6" s="11">
+      <c r="R6" s="9">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S6" s="9">
         <f t="shared" si="6"/>
         <v>16.583333333333332</v>
       </c>
@@ -2027,11 +2032,11 @@
       <c r="W6" s="2">
         <v>45358</v>
       </c>
-      <c r="X6" s="11">
+      <c r="X6" s="9">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Y6" s="9">
         <f t="shared" si="8"/>
         <v>16.583333333333332</v>
       </c>
@@ -2049,20 +2054,20 @@
       </c>
       <c r="B7" s="4">
         <f>SUM(B3:B6)</f>
-        <v>81.733333333333391</v>
+        <v>88.066666666666734</v>
       </c>
       <c r="C7" s="6">
         <f>SUM(C3:C6)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="E7" s="2">
         <v>45316</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f>19+42/60</f>
         <v>19.7</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <f xml:space="preserve"> 21 + 30/60</f>
         <v>21.5</v>
       </c>
@@ -2076,10 +2081,10 @@
       <c r="K7" s="2">
         <v>45335</v>
       </c>
-      <c r="L7" s="11">
-        <v>8</v>
-      </c>
-      <c r="M7" s="11">
+      <c r="L7" s="9">
+        <v>8</v>
+      </c>
+      <c r="M7" s="9">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2093,11 +2098,11 @@
       <c r="Q7" s="2">
         <v>45365</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="9">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="9">
         <f t="shared" si="6"/>
         <v>16.583333333333332</v>
       </c>
@@ -2111,11 +2116,11 @@
       <c r="W7" s="2">
         <v>45365</v>
       </c>
-      <c r="X7" s="11">
+      <c r="X7" s="9">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="Y7" s="9">
         <f t="shared" si="8"/>
         <v>16.583333333333332</v>
       </c>
@@ -2131,11 +2136,11 @@
       <c r="E8" s="2">
         <v>45321</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2149,10 +2154,10 @@
       <c r="K8" s="2">
         <v>45336</v>
       </c>
-      <c r="L8" s="11">
-        <v>8</v>
-      </c>
-      <c r="M8" s="11">
+      <c r="L8" s="9">
+        <v>8</v>
+      </c>
+      <c r="M8" s="9">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2166,11 +2171,11 @@
       <c r="Q8" s="2">
         <v>45393</v>
       </c>
-      <c r="R8" s="11">
+      <c r="R8" s="9">
         <f>18+45/60</f>
         <v>18.75</v>
       </c>
-      <c r="S8" s="11">
+      <c r="S8" s="9">
         <f>19+15/60</f>
         <v>19.25</v>
       </c>
@@ -2184,11 +2189,11 @@
       <c r="W8" s="2">
         <v>45393</v>
       </c>
-      <c r="X8" s="11">
+      <c r="X8" s="9">
         <f>19+15/60</f>
         <v>19.25</v>
       </c>
-      <c r="Y8" s="11">
+      <c r="Y8" s="9">
         <f>19+53/60</f>
         <v>19.883333333333333</v>
       </c>
@@ -2204,11 +2209,11 @@
       <c r="E9" s="2">
         <v>45322</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <f>14+45/60</f>
         <v>14.75</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
         <f>16+40/60</f>
         <v>16.666666666666668</v>
       </c>
@@ -2222,11 +2227,11 @@
       <c r="K9" s="2">
         <v>45342</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="9">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2252,10 +2257,10 @@
       <c r="E10" s="2">
         <v>45323</v>
       </c>
-      <c r="F10" s="11">
-        <v>8</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="F10" s="9">
+        <v>8</v>
+      </c>
+      <c r="G10" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2269,11 +2274,11 @@
       <c r="K10" s="2">
         <v>45343</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="9">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2299,11 +2304,11 @@
       <c r="E11" s="2">
         <v>45323</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <f>17+35/60</f>
         <v>17.583333333333332</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <f>19</f>
         <v>19</v>
       </c>
@@ -2317,11 +2322,11 @@
       <c r="K11" s="2">
         <v>45349</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="9">
         <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2347,11 +2352,11 @@
       <c r="E12" s="2">
         <v>45324</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2365,10 +2370,10 @@
       <c r="K12" s="2">
         <v>45356</v>
       </c>
-      <c r="L12" s="11">
-        <v>8</v>
-      </c>
-      <c r="M12" s="11">
+      <c r="L12" s="9">
+        <v>8</v>
+      </c>
+      <c r="M12" s="9">
         <f t="shared" ref="M12:M18" si="9">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2394,11 +2399,11 @@
       <c r="E13" s="2">
         <v>45324</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <f>13+53/60</f>
         <v>13.883333333333333</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="9">
         <f>14+36/60</f>
         <v>14.6</v>
       </c>
@@ -2412,11 +2417,11 @@
       <c r="K13" s="2">
         <v>45363</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="9">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2442,11 +2447,11 @@
       <c r="E14" s="2">
         <v>45326</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <f xml:space="preserve"> 18+30/60</f>
         <v>18.5</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="9">
         <f>19+42/60</f>
         <v>19.7</v>
       </c>
@@ -2460,11 +2465,11 @@
       <c r="K14" s="2">
         <v>45384</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="9">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2490,11 +2495,11 @@
       <c r="E15" s="2">
         <v>45334</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="9">
         <f>12+53/60</f>
         <v>12.883333333333333</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="9">
         <f>13+7/60</f>
         <v>13.116666666666667</v>
       </c>
@@ -2508,11 +2513,11 @@
       <c r="K15" s="2">
         <v>45385</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="9">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2538,11 +2543,11 @@
       <c r="E16" s="2">
         <v>45334</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="9">
         <f>10+21/60</f>
         <v>10.35</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="9">
         <f>10+42/60</f>
         <v>10.7</v>
       </c>
@@ -2556,11 +2561,11 @@
       <c r="K16" s="2">
         <v>45391</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="9">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2582,14 +2587,14 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E17" s="2">
         <v>45335</v>
       </c>
-      <c r="F17" s="11">
-        <v>8</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="F17" s="9">
+        <v>8</v>
+      </c>
+      <c r="G17" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2603,11 +2608,11 @@
       <c r="K17" s="2">
         <v>45392</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="9">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2629,15 +2634,15 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E18" s="2">
         <v>45335</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="9">
         <f>14+32/60</f>
         <v>14.533333333333333</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="9">
         <f>15 + 10/60</f>
         <v>15.166666666666666</v>
       </c>
@@ -2651,11 +2656,11 @@
       <c r="K18" s="2">
         <v>45399</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="9">
         <f t="shared" si="9"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2677,15 +2682,15 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E19" s="2">
         <v>45335</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="9">
         <f>17+35/60</f>
         <v>17.583333333333332</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="9">
         <f>17+47/60</f>
         <v>17.783333333333335</v>
       </c>
@@ -2699,11 +2704,11 @@
       <c r="K19" s="2">
         <v>45399</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="9">
         <f>20+33/60</f>
         <v>20.55</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="9">
         <f>21+12/60</f>
         <v>21.2</v>
       </c>
@@ -2725,14 +2730,14 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E20" s="2">
         <v>45336</v>
       </c>
-      <c r="F20" s="11">
-        <v>8</v>
-      </c>
-      <c r="G20" s="11">
+      <c r="F20" s="9">
+        <v>8</v>
+      </c>
+      <c r="G20" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2744,12 +2749,12 @@
       <c r="K20" s="2">
         <v>45405</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M20" s="11">
-        <f t="shared" ref="M20:M21" si="13">9+35/60</f>
+      <c r="M20" s="9">
+        <f t="shared" ref="M20:M23" si="13">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="N20" s="3">
@@ -2770,15 +2775,15 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E21" s="2">
         <v>45342</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2792,11 +2797,11 @@
       <c r="K21" s="2">
         <v>45406</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M21" s="9">
         <f t="shared" si="13"/>
         <v>9.5833333333333339</v>
       </c>
@@ -2818,15 +2823,15 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E22" s="2">
         <v>45343</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2837,14 +2842,24 @@
       <c r="I22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="K22" s="2">
+        <v>45419</v>
+      </c>
+      <c r="L22" s="9">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M22" s="9">
+        <f t="shared" si="13"/>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="N22" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="1"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2856,15 +2871,15 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E23" s="2">
         <v>45349</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2873,14 +2888,24 @@
         <v>1.5833333333333339</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="K23" s="2">
+        <v>45420</v>
+      </c>
+      <c r="L23" s="9">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M23" s="9">
+        <f t="shared" si="13"/>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="N23" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="1"/>
+        <f t="shared" ref="N23" si="14">M23-L23</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -2892,15 +2917,15 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E24" s="2">
         <v>45350</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="9">
         <f>18+24/60</f>
         <v>18.399999999999999</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="9">
         <f>20+21/60</f>
         <v>20.350000000000001</v>
       </c>
@@ -2928,15 +2953,15 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E25" s="2">
         <v>45352</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="9">
         <f>14+54/60</f>
         <v>14.9</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="9">
         <f>16+22/60</f>
         <v>16.366666666666667</v>
       </c>
@@ -2953,15 +2978,15 @@
       <c r="N25" s="2"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E26" s="2">
         <v>45356</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2978,20 +3003,20 @@
       <c r="N26" s="2"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E27" s="2">
         <v>45357</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="9">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" ref="H27:H34" si="14">G27-F27</f>
+        <f t="shared" ref="H27:H34" si="15">G27-F27</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -3003,20 +3028,20 @@
       <c r="N27" s="2"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E28" s="2">
         <v>45357</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="9">
         <f>17+54/60</f>
         <v>17.899999999999999</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="9">
         <f>18+31/60</f>
         <v>18.516666666666666</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.61666666666666714</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -3028,80 +3053,81 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E29" s="2">
         <v>45359</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="9">
         <f>15+53/60</f>
         <v>15.883333333333333</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="9">
         <f>16+29/60</f>
         <v>16.483333333333334</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E30" s="2">
         <v>45361</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="9">
         <f>16+42/60</f>
         <v>16.7</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="9">
         <f>17+10/60</f>
         <v>17.166666666666668</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.46666666666666856</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
       <c r="E31" s="2">
         <v>45363</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G31" s="11">
-        <f t="shared" ref="G31:G38" si="15">9+35/60</f>
+      <c r="G31" s="9">
+        <f t="shared" ref="G31:G40" si="16">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E32" s="2">
         <v>45384</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="9">
+        <f t="shared" si="16"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H32" s="3">
         <f t="shared" si="15"/>
-        <v>9.5833333333333339</v>
-      </c>
-      <c r="H32" s="3">
-        <f t="shared" si="14"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -3112,16 +3138,16 @@
       <c r="E33" s="2">
         <v>45385</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="9">
+        <f t="shared" si="16"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H33" s="3">
         <f t="shared" si="15"/>
-        <v>9.5833333333333339</v>
-      </c>
-      <c r="H33" s="3">
-        <f t="shared" si="14"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -3132,16 +3158,16 @@
       <c r="E34" s="2">
         <v>45391</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="9">
+        <f t="shared" si="16"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H34" s="3">
         <f t="shared" si="15"/>
-        <v>9.5833333333333339</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="14"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -3152,16 +3178,16 @@
       <c r="E35" s="2">
         <v>45392</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G35" s="11">
-        <f t="shared" si="15"/>
+      <c r="G35" s="9">
+        <f t="shared" si="16"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" ref="H35" si="16">G35-F35</f>
+        <f t="shared" ref="H35" si="17">G35-F35</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -3172,16 +3198,16 @@
       <c r="E36" s="2">
         <v>45399</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G36" s="11">
-        <f t="shared" si="15"/>
+      <c r="G36" s="9">
+        <f t="shared" si="16"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" ref="H36" si="17">G36-F36</f>
+        <f t="shared" ref="H36" si="18">G36-F36</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -3192,19 +3218,19 @@
       <c r="E37" s="2">
         <v>45405</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G37" s="11">
-        <f t="shared" si="15"/>
+      <c r="G37" s="9">
+        <f t="shared" si="16"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" ref="H37:H38" si="18">G37-F37</f>
-        <v>1.5833333333333339</v>
-      </c>
-      <c r="I37" s="10" t="s">
+        <f t="shared" ref="H37:H39" si="19">G37-F37</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3212,16 +3238,16 @@
       <c r="E38" s="2">
         <v>45406</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="9">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="G38" s="11">
-        <f t="shared" si="15"/>
+      <c r="G38" s="9">
+        <f t="shared" si="16"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -3229,18 +3255,44 @@
       </c>
     </row>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="E39" s="2">
+        <v>45419</v>
+      </c>
+      <c r="F39" s="9">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G39" s="9">
+        <f t="shared" si="16"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" si="19"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="E40" s="2">
+        <v>45420</v>
+      </c>
+      <c r="F40" s="9">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G40" s="9">
+        <f t="shared" si="16"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H40" s="3">
+        <f t="shared" ref="H40" si="20">G40-F40</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>

</xml_diff>

<commit_message>
new build + font_colour main menu
</commit_message>
<xml_diff>
--- a/Buerokratie/PM/timeLog.xlsx
+++ b/Buerokratie/PM/timeLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\Buerokratie\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C395D3-6FD5-4C72-B5A7-579C1EF9123A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B570775-CE1C-4E35-AE61-2B6F92A6C1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Begin</t>
   </si>
@@ -167,33 +167,9 @@
     <t>bug fixes ._.</t>
   </si>
   <si>
-    <t>Steffi</t>
-  </si>
-  <si>
-    <t>Elina</t>
-  </si>
-  <si>
     <t>Summe</t>
   </si>
   <si>
-    <t>Erklärung des Projekts</t>
-  </si>
-  <si>
-    <t>Planung der Vorgangsweise</t>
-  </si>
-  <si>
-    <t>Projektantrag</t>
-  </si>
-  <si>
-    <t>OSP</t>
-  </si>
-  <si>
-    <t>PSP</t>
-  </si>
-  <si>
-    <t>Zeitplan</t>
-  </si>
-  <si>
     <t>Bürokratie</t>
   </si>
   <si>
@@ -204,6 +180,18 @@
   </si>
   <si>
     <t>tries counter</t>
+  </si>
+  <si>
+    <t>Küchenhintergrund</t>
+  </si>
+  <si>
+    <t>playtesting + fixes</t>
+  </si>
+  <si>
+    <t>dont reset music on rest + itch.io page</t>
+  </si>
+  <si>
+    <t>Küche</t>
   </si>
 </sst>
 </file>
@@ -267,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -275,8 +263,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,85 +402,31 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-F689-4C9B-B8B2-116F3F9503F5}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-F689-4C9B-B8B2-116F3F9503F5}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$3:$A$6</c:f>
+              <c:f>Tabelle1!$A$3:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Viki</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Aris</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Steffi</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Elina</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$B$6</c:f>
+              <c:f>Tabelle1!$B$3:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "h"</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>30.816666666666691</c:v>
+                  <c:v>33.983333333333363</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.283333333333388</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.4166666666666607</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.5499999999999936</c:v>
+                  <c:v>53.45000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -548,85 +480,31 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-F689-4C9B-B8B2-116F3F9503F5}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000F-F689-4C9B-B8B2-116F3F9503F5}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$3:$A$6</c:f>
+              <c:f>Tabelle1!$A$3:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Viki</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Aris</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Steffi</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Elina</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$3:$C$6</c:f>
+              <c:f>Tabelle1!$C$3:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.34992429977289935</c:v>
+                  <c:v>0.38867708730461298</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57096896290688892</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>3.8796366389099071E-2</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0%">
-                  <c:v>4.0310370931112692E-2</c:v>
+                  <c:v>0.61132291269538697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,13 +1171,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>310931</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>47295</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3004206</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>122620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1591,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA45"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1483,7 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="87.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
@@ -1622,25 +1500,19 @@
     <col min="27" max="27" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="8"/>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>31</v>
       </c>
@@ -1677,57 +1549,27 @@
       <c r="O2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4">
         <f>SUM(N3:N41)</f>
-        <v>30.816666666666691</v>
+        <v>33.983333333333363</v>
       </c>
       <c r="C3" s="5">
-        <f>B3/B7</f>
-        <v>0.34992429977289935</v>
+        <f>B3/B5</f>
+        <v>0.38867708730461298</v>
       </c>
       <c r="E3" s="2">
         <v>45314</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <f>8 + 45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1741,78 +1583,42 @@
       <c r="K3" s="2">
         <v>45314</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="7">
         <f>8 + 45/60</f>
         <v>8.75</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="7">
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N24" si="1">M3-L3</f>
+        <f t="shared" ref="N3:N22" si="1">M3-L3</f>
         <v>0.83333333333333393</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="2">
-        <v>45344</v>
-      </c>
-      <c r="R3" s="9">
-        <f>16+0/60</f>
-        <v>16</v>
-      </c>
-      <c r="S3" s="9">
-        <f>16+35/60</f>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="T3" s="8">
-        <f t="shared" ref="T3:T8" si="2">S3-R3</f>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W3" s="2">
-        <v>45344</v>
-      </c>
-      <c r="X3" s="9">
-        <f>16+0/60</f>
-        <v>16</v>
-      </c>
-      <c r="Y3" s="9">
-        <f>16+35/60</f>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="Z3" s="8">
-        <f t="shared" ref="Z3:Z8" si="3">Y3-X3</f>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4">
         <f>SUM(H3:H64)</f>
-        <v>50.283333333333388</v>
+        <v>53.45000000000006</v>
       </c>
       <c r="C4" s="5">
-        <f>B4/B7</f>
-        <v>0.57096896290688892</v>
+        <f>B4/B5</f>
+        <v>0.61132291269538697</v>
       </c>
       <c r="E4" s="2">
         <v>45314</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <f>18+37/60</f>
         <v>18.616666666666667</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <f>21 + 20/60</f>
         <v>21.333333333333332</v>
       </c>
@@ -1827,12 +1633,12 @@
       <c r="K4" s="2">
         <v>45315</v>
       </c>
-      <c r="L4" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M4" s="9">
-        <f t="shared" ref="M4:M11" si="4">9+35/60</f>
+      <c r="L4" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M4" s="7">
+        <f t="shared" ref="M4:M11" si="2">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="N4" s="3">
@@ -1842,63 +1648,27 @@
       <c r="O4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="2">
-        <v>45351</v>
-      </c>
-      <c r="R4" s="9">
-        <f t="shared" ref="R4:R7" si="5">16+0/60</f>
-        <v>16</v>
-      </c>
-      <c r="S4" s="9">
-        <f t="shared" ref="S4:S7" si="6">16+35/60</f>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="T4" s="8">
-        <f t="shared" si="2"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W4" s="2">
-        <v>45351</v>
-      </c>
-      <c r="X4" s="9">
-        <f t="shared" ref="X4:X7" si="7">16+0/60</f>
-        <v>16</v>
-      </c>
-      <c r="Y4" s="9">
-        <f t="shared" ref="Y4:Y7" si="8">16+35/60</f>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="Z4" s="8">
-        <f t="shared" si="3"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="4">
-        <f>SUM(T3:T77)</f>
-        <v>3.4166666666666607</v>
-      </c>
-      <c r="C5" s="7">
-        <f>B5/B7</f>
-        <v>3.8796366389099071E-2</v>
+        <f>SUM(B3:B4)</f>
+        <v>87.433333333333422</v>
+      </c>
+      <c r="C5" s="6">
+        <f>SUM(C3:C4)</f>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>45315</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <f>11 + 10/60</f>
         <v>11.166666666666666</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <f xml:space="preserve"> 13</f>
         <v>13</v>
       </c>
@@ -1912,12 +1682,12 @@
       <c r="K5" s="2">
         <v>45321</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="7">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="M5" s="9">
-        <f t="shared" si="4"/>
+      <c r="M5" s="7">
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N5" s="3">
@@ -1927,63 +1697,16 @@
       <c r="O5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="2">
-        <v>45358</v>
-      </c>
-      <c r="R5" s="9">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="S5" s="9">
-        <f t="shared" si="6"/>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="T5" s="8">
-        <f t="shared" si="2"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="W5" s="2">
-        <v>45358</v>
-      </c>
-      <c r="X5" s="9">
-        <f t="shared" si="7"/>
-        <v>16</v>
-      </c>
-      <c r="Y5" s="9">
-        <f t="shared" si="8"/>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="Z5" s="8">
-        <f t="shared" si="3"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="4">
-        <f>SUM(Z3:Z95)</f>
-        <v>3.5499999999999936</v>
-      </c>
-      <c r="C6" s="7">
-        <f>B6/B7</f>
-        <v>4.0310370931112692E-2</v>
-      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E6" s="2">
         <v>45315</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <f xml:space="preserve"> 17 + 30/60</f>
         <v>17.5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <f>18 + 40/60</f>
         <v>18.666666666666668</v>
       </c>
@@ -1997,11 +1720,11 @@
       <c r="K6" s="2">
         <v>45322</v>
       </c>
-      <c r="L6" s="9">
-        <v>8</v>
-      </c>
-      <c r="M6" s="9">
-        <f t="shared" si="4"/>
+      <c r="L6" s="7">
+        <v>8</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N6" s="3">
@@ -2011,63 +1734,16 @@
       <c r="O6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="2">
-        <v>45358</v>
-      </c>
-      <c r="R6" s="9">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="S6" s="9">
-        <f t="shared" si="6"/>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="T6" s="8">
-        <f t="shared" si="2"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W6" s="2">
-        <v>45358</v>
-      </c>
-      <c r="X6" s="9">
-        <f t="shared" si="7"/>
-        <v>16</v>
-      </c>
-      <c r="Y6" s="9">
-        <f t="shared" si="8"/>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="Z6" s="8">
-        <f t="shared" si="3"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="4">
-        <f>SUM(B3:B6)</f>
-        <v>88.066666666666734</v>
-      </c>
-      <c r="C7" s="6">
-        <f>SUM(C3:C6)</f>
-        <v>1.0000000000000002</v>
-      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E7" s="2">
         <v>45316</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <f>19+42/60</f>
         <v>19.7</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <f xml:space="preserve"> 21 + 30/60</f>
         <v>21.5</v>
       </c>
@@ -2081,11 +1757,11 @@
       <c r="K7" s="2">
         <v>45335</v>
       </c>
-      <c r="L7" s="9">
-        <v>8</v>
-      </c>
-      <c r="M7" s="9">
-        <f t="shared" si="4"/>
+      <c r="L7" s="7">
+        <v>8</v>
+      </c>
+      <c r="M7" s="7">
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N7" s="3">
@@ -2095,52 +1771,16 @@
       <c r="O7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="2">
-        <v>45365</v>
-      </c>
-      <c r="R7" s="9">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="S7" s="9">
-        <f t="shared" si="6"/>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="T7" s="8">
-        <f t="shared" si="2"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W7" s="2">
-        <v>45365</v>
-      </c>
-      <c r="X7" s="9">
-        <f t="shared" si="7"/>
-        <v>16</v>
-      </c>
-      <c r="Y7" s="9">
-        <f t="shared" si="8"/>
-        <v>16.583333333333332</v>
-      </c>
-      <c r="Z7" s="8">
-        <f t="shared" si="3"/>
-        <v>0.58333333333333215</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E8" s="2">
         <v>45321</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2154,11 +1794,11 @@
       <c r="K8" s="2">
         <v>45336</v>
       </c>
-      <c r="L8" s="9">
-        <v>8</v>
-      </c>
-      <c r="M8" s="9">
-        <f t="shared" si="4"/>
+      <c r="L8" s="7">
+        <v>8</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N8" s="3">
@@ -2168,52 +1808,16 @@
       <c r="O8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="2">
-        <v>45393</v>
-      </c>
-      <c r="R8" s="9">
-        <f>18+45/60</f>
-        <v>18.75</v>
-      </c>
-      <c r="S8" s="9">
-        <f>19+15/60</f>
-        <v>19.25</v>
-      </c>
-      <c r="T8" s="8">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="W8" s="2">
-        <v>45393</v>
-      </c>
-      <c r="X8" s="9">
-        <f>19+15/60</f>
-        <v>19.25</v>
-      </c>
-      <c r="Y8" s="9">
-        <f>19+53/60</f>
-        <v>19.883333333333333</v>
-      </c>
-      <c r="Z8" s="8">
-        <f t="shared" si="3"/>
-        <v>0.63333333333333286</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E9" s="2">
         <v>45322</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <f>14+45/60</f>
         <v>14.75</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <f>16+40/60</f>
         <v>16.666666666666668</v>
       </c>
@@ -2227,12 +1831,12 @@
       <c r="K9" s="2">
         <v>45342</v>
       </c>
-      <c r="L9" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M9" s="9">
-        <f t="shared" si="4"/>
+      <c r="L9" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M9" s="7">
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N9" s="3">
@@ -2242,25 +1846,15 @@
       <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E10" s="2">
         <v>45323</v>
       </c>
-      <c r="F10" s="9">
-        <v>8</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="F10" s="7">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2274,12 +1868,12 @@
       <c r="K10" s="2">
         <v>45343</v>
       </c>
-      <c r="L10" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M10" s="9">
-        <f t="shared" si="4"/>
+      <c r="L10" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M10" s="7">
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N10" s="3">
@@ -2289,26 +1883,16 @@
       <c r="O10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E11" s="2">
         <v>45323</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <f>17+35/60</f>
         <v>17.583333333333332</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <f>19</f>
         <v>19</v>
       </c>
@@ -2322,12 +1906,12 @@
       <c r="K11" s="2">
         <v>45349</v>
       </c>
-      <c r="L11" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M11" s="9">
-        <f t="shared" si="4"/>
+      <c r="L11" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M11" s="7">
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N11" s="3">
@@ -2337,26 +1921,16 @@
       <c r="O11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E12" s="2">
         <v>45324</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <f>8+45/60</f>
         <v>8.75</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2370,11 +1944,11 @@
       <c r="K12" s="2">
         <v>45356</v>
       </c>
-      <c r="L12" s="9">
-        <v>8</v>
-      </c>
-      <c r="M12" s="9">
-        <f t="shared" ref="M12:M18" si="9">9+35/60</f>
+      <c r="L12" s="7">
+        <v>8</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" ref="M12:M18" si="3">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="N12" s="3">
@@ -2384,26 +1958,16 @@
       <c r="O12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E13" s="2">
         <v>45324</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <f>13+53/60</f>
         <v>13.883333333333333</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <f>14+36/60</f>
         <v>14.6</v>
       </c>
@@ -2417,41 +1981,31 @@
       <c r="K13" s="2">
         <v>45363</v>
       </c>
-      <c r="L13" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M13" s="9">
-        <f t="shared" si="9"/>
+      <c r="L13" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" si="3"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" ref="N13" si="10">M13-L13</f>
+        <f t="shared" ref="N13" si="4">M13-L13</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E14" s="2">
         <v>45326</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <f xml:space="preserve"> 18+30/60</f>
         <v>18.5</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <f>19+42/60</f>
         <v>19.7</v>
       </c>
@@ -2465,12 +2019,12 @@
       <c r="K14" s="2">
         <v>45384</v>
       </c>
-      <c r="L14" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M14" s="9">
-        <f t="shared" si="9"/>
+      <c r="L14" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="3"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N14" s="3">
@@ -2480,26 +2034,16 @@
       <c r="O14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E15" s="2">
         <v>45334</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <f>12+53/60</f>
         <v>12.883333333333333</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <f>13+7/60</f>
         <v>13.116666666666667</v>
       </c>
@@ -2513,12 +2057,12 @@
       <c r="K15" s="2">
         <v>45385</v>
       </c>
-      <c r="L15" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M15" s="9">
-        <f t="shared" si="9"/>
+      <c r="L15" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M15" s="7">
+        <f t="shared" si="3"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N15" s="3">
@@ -2528,26 +2072,16 @@
       <c r="O15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E16" s="2">
         <v>45334</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <f>10+21/60</f>
         <v>10.35</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <f>10+42/60</f>
         <v>10.7</v>
       </c>
@@ -2561,12 +2095,12 @@
       <c r="K16" s="2">
         <v>45391</v>
       </c>
-      <c r="L16" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M16" s="9">
-        <f t="shared" si="9"/>
+      <c r="L16" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M16" s="7">
+        <f t="shared" si="3"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N16" s="3">
@@ -2576,25 +2110,15 @@
       <c r="O16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="3:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E17" s="2">
         <v>45335</v>
       </c>
-      <c r="F17" s="9">
-        <v>8</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="F17" s="7">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2608,41 +2132,31 @@
       <c r="K17" s="2">
         <v>45392</v>
       </c>
-      <c r="L17" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M17" s="9">
-        <f t="shared" si="9"/>
+      <c r="L17" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M17" s="7">
+        <f t="shared" si="3"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" ref="N17" si="11">M17-L17</f>
+        <f t="shared" ref="N17" si="5">M17-L17</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-    </row>
-    <row r="18" spans="3:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E18" s="2">
         <v>45335</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <f>14+32/60</f>
         <v>14.533333333333333</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <f>15 + 10/60</f>
         <v>15.166666666666666</v>
       </c>
@@ -2656,41 +2170,31 @@
       <c r="K18" s="2">
         <v>45399</v>
       </c>
-      <c r="L18" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M18" s="9">
-        <f t="shared" si="9"/>
+      <c r="L18" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M18" s="7">
+        <f t="shared" si="3"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" ref="N18" si="12">M18-L18</f>
+        <f t="shared" ref="N18" si="6">M18-L18</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-    </row>
-    <row r="19" spans="3:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E19" s="2">
         <v>45335</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <f>17+35/60</f>
         <v>17.583333333333332</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <f>17+47/60</f>
         <v>17.783333333333335</v>
       </c>
@@ -2704,11 +2208,11 @@
       <c r="K19" s="2">
         <v>45399</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="7">
         <f>20+33/60</f>
         <v>20.55</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="7">
         <f>21+12/60</f>
         <v>21.2</v>
       </c>
@@ -2717,27 +2221,17 @@
         <v>0.64999999999999858</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-    </row>
-    <row r="20" spans="3:27" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E20" s="2">
         <v>45336</v>
       </c>
-      <c r="F20" s="9">
-        <v>8</v>
-      </c>
-      <c r="G20" s="9">
+      <c r="F20" s="7">
+        <v>8</v>
+      </c>
+      <c r="G20" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2749,12 +2243,12 @@
       <c r="K20" s="2">
         <v>45405</v>
       </c>
-      <c r="L20" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M20" s="9">
-        <f t="shared" ref="M20:M23" si="13">9+35/60</f>
+      <c r="L20" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" ref="M20:M25" si="7">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="N20" s="3">
@@ -2764,26 +2258,16 @@
       <c r="O20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-    </row>
-    <row r="21" spans="3:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E21" s="2">
         <v>45342</v>
       </c>
-      <c r="F21" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G21" s="9">
+      <c r="F21" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G21" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2797,12 +2281,12 @@
       <c r="K21" s="2">
         <v>45406</v>
       </c>
-      <c r="L21" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M21" s="9">
-        <f t="shared" si="13"/>
+      <c r="L21" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M21" s="7">
+        <f t="shared" si="7"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N21" s="3">
@@ -2812,26 +2296,16 @@
       <c r="O21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-    </row>
-    <row r="22" spans="3:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E22" s="2">
         <v>45343</v>
       </c>
-      <c r="F22" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G22" s="9">
+      <c r="F22" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G22" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2845,12 +2319,12 @@
       <c r="K22" s="2">
         <v>45419</v>
       </c>
-      <c r="L22" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M22" s="9">
-        <f t="shared" si="13"/>
+      <c r="L22" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M22" s="7">
+        <f t="shared" si="7"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N22" s="3">
@@ -2860,26 +2334,16 @@
       <c r="O22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-    </row>
-    <row r="23" spans="3:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E23" s="2">
         <v>45349</v>
       </c>
-      <c r="F23" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G23" s="9">
+      <c r="F23" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G23" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -2891,41 +2355,31 @@
       <c r="K23" s="2">
         <v>45420</v>
       </c>
-      <c r="L23" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="M23" s="9">
-        <f t="shared" si="13"/>
+      <c r="L23" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M23" s="7">
+        <f t="shared" si="7"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" ref="N23" si="14">M23-L23</f>
+        <f t="shared" ref="N23:N24" si="8">M23-L23</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-    </row>
-    <row r="24" spans="3:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E24" s="2">
         <v>45350</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <f>18+24/60</f>
         <v>18.399999999999999</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="7">
         <f>20+21/60</f>
         <v>20.350000000000001</v>
       </c>
@@ -2934,34 +2388,34 @@
         <v>1.9500000000000028</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="K24" s="2">
+        <v>45426</v>
+      </c>
+      <c r="L24" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M24" s="7">
+        <f t="shared" si="7"/>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="N24" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-    </row>
-    <row r="25" spans="3:27" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E25" s="2">
         <v>45352</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="7">
         <f>14+54/60</f>
         <v>14.9</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="7">
         <f>16+22/60</f>
         <v>16.366666666666667</v>
       </c>
@@ -2972,21 +2426,34 @@
       <c r="I25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="K25" s="2">
+        <v>45427</v>
+      </c>
+      <c r="L25" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="M25" s="7">
+        <f t="shared" si="7"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" ref="N25" si="9">M25-L25</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E26" s="2">
         <v>45356</v>
       </c>
-      <c r="F26" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="F26" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G26" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -3003,20 +2470,20 @@
       <c r="N26" s="2"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E27" s="2">
         <v>45357</v>
       </c>
-      <c r="F27" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G27" s="9">
+      <c r="F27" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G27" s="7">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" ref="H27:H34" si="15">G27-F27</f>
+        <f t="shared" ref="H27:H34" si="10">G27-F27</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -3028,20 +2495,20 @@
       <c r="N27" s="2"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E28" s="2">
         <v>45357</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="7">
         <f>17+54/60</f>
         <v>17.899999999999999</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <f>18+31/60</f>
         <v>18.516666666666666</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>0.61666666666666714</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -3053,81 +2520,81 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
       <c r="E29" s="2">
         <v>45359</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <f>15+53/60</f>
         <v>15.883333333333333</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <f>16+29/60</f>
         <v>16.483333333333334</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E30" s="2">
         <v>45361</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <f>16+42/60</f>
         <v>16.7</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <f>17+10/60</f>
         <v>17.166666666666668</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>0.46666666666666856</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C31" s="6"/>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E31" s="2">
         <v>45363</v>
       </c>
-      <c r="F31" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G31" s="9">
-        <f t="shared" ref="G31:G40" si="16">9+35/60</f>
+      <c r="F31" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" ref="G31:G42" si="11">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E32" s="2">
         <v>45384</v>
       </c>
-      <c r="F32" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G32" s="9">
-        <f t="shared" si="16"/>
+      <c r="F32" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G32" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -3138,16 +2605,16 @@
       <c r="E33" s="2">
         <v>45385</v>
       </c>
-      <c r="F33" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G33" s="9">
-        <f t="shared" si="16"/>
+      <c r="F33" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G33" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -3158,16 +2625,16 @@
       <c r="E34" s="2">
         <v>45391</v>
       </c>
-      <c r="F34" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G34" s="9">
-        <f t="shared" si="16"/>
+      <c r="F34" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G34" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -3178,16 +2645,16 @@
       <c r="E35" s="2">
         <v>45392</v>
       </c>
-      <c r="F35" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G35" s="9">
-        <f t="shared" si="16"/>
+      <c r="F35" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G35" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" ref="H35" si="17">G35-F35</f>
+        <f t="shared" ref="H35" si="12">G35-F35</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -3198,16 +2665,16 @@
       <c r="E36" s="2">
         <v>45399</v>
       </c>
-      <c r="F36" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G36" s="9">
-        <f t="shared" si="16"/>
+      <c r="F36" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G36" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" ref="H36" si="18">G36-F36</f>
+        <f t="shared" ref="H36" si="13">G36-F36</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -3218,36 +2685,36 @@
       <c r="E37" s="2">
         <v>45405</v>
       </c>
-      <c r="F37" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G37" s="9">
-        <f t="shared" si="16"/>
+      <c r="F37" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G37" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" ref="H37:H39" si="19">G37-F37</f>
+        <f t="shared" ref="H37:H39" si="14">G37-F37</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E38" s="2">
         <v>45406</v>
       </c>
-      <c r="F38" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G38" s="9">
-        <f t="shared" si="16"/>
+      <c r="F38" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G38" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -3258,55 +2725,81 @@
       <c r="E39" s="2">
         <v>45419</v>
       </c>
-      <c r="F39" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G39" s="9">
-        <f t="shared" si="16"/>
+      <c r="F39" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G39" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E40" s="2">
         <v>45420</v>
       </c>
-      <c r="F40" s="9">
-        <f>8</f>
-        <v>8</v>
-      </c>
-      <c r="G40" s="9">
-        <f t="shared" si="16"/>
+      <c r="F40" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G40" s="7">
+        <f t="shared" si="11"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="H40" s="3">
-        <f t="shared" ref="H40" si="20">G40-F40</f>
+        <f t="shared" ref="H40" si="15">G40-F40</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="E41" s="2">
+        <v>45426</v>
+      </c>
+      <c r="F41" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G41" s="7">
+        <f t="shared" si="11"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H41" s="3">
+        <f t="shared" ref="H41" si="16">G41-F41</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="E42" s="2">
+        <v>45427</v>
+      </c>
+      <c r="F42" s="7">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="G42" s="7">
+        <f t="shared" si="11"/>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="H42" s="3">
+        <f t="shared" ref="H42" si="17">G42-F42</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E43" s="1"/>

</xml_diff>